<commit_message>
Run Test Suite wolfssl
</commit_message>
<xml_diff>
--- a/ExcelFiles/FFmpeg_Select.xlsx
+++ b/ExcelFiles/FFmpeg_Select.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyeedahmed/Desktop/Gitcode/LLMVerification/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19DD513-346E-D84D-BABB-0ECAEC91CAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE98523-668B-A04D-B4DF-A5B78650E71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="500" windowWidth="16940" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="-28300" windowWidth="26780" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commits" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="250">
   <si>
     <t>Commit Date</t>
   </si>
@@ -847,14 +847,20 @@
   <si>
     <t>enc_open</t>
   </si>
+  <si>
+    <t>Test_Suite</t>
+  </si>
+  <si>
+    <t>TestSuite</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -881,7 +887,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -904,17 +910,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1219,19 +1239,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1245,28 +1267,31 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40939</v>
       </c>
@@ -1280,22 +1305,22 @@
         <v>104</v>
       </c>
       <c r="E2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>142</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>146</v>
       </c>
-      <c r="I2">
-        <v>11</v>
-      </c>
-      <c r="J2">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40939</v>
       </c>
@@ -1309,22 +1334,22 @@
         <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" t="s">
         <v>146</v>
       </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>39</v>
-      </c>
-      <c r="K3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>41181</v>
       </c>
@@ -1338,25 +1363,25 @@
         <v>105</v>
       </c>
       <c r="E4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
         <v>140</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>146</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>153</v>
       </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>37</v>
-      </c>
-      <c r="K4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>41618</v>
       </c>
@@ -1370,22 +1395,22 @@
         <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" t="s">
         <v>146</v>
       </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>41992</v>
       </c>
@@ -1399,25 +1424,25 @@
         <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" t="s">
         <v>149</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>154</v>
       </c>
-      <c r="I6">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42059</v>
       </c>
@@ -1431,22 +1456,22 @@
         <v>108</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" t="s">
         <v>150</v>
       </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-      <c r="K7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42059</v>
       </c>
@@ -1460,22 +1485,22 @@
         <v>109</v>
       </c>
       <c r="E8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8">
+        <v>48</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>141</v>
+      </c>
+      <c r="I8" t="s">
         <v>150</v>
       </c>
-      <c r="I8">
-        <v>48</v>
-      </c>
-      <c r="J8">
-        <v>11</v>
-      </c>
-      <c r="K8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42059</v>
       </c>
@@ -1489,22 +1514,22 @@
         <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" t="s">
         <v>150</v>
       </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>8</v>
-      </c>
-      <c r="K9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42063</v>
       </c>
@@ -1518,22 +1543,22 @@
         <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I10" t="s">
         <v>148</v>
       </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>8</v>
-      </c>
-      <c r="K10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>42063</v>
       </c>
@@ -1547,22 +1572,22 @@
         <v>111</v>
       </c>
       <c r="E11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
         <v>140</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>147</v>
       </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11">
-        <v>7</v>
-      </c>
-      <c r="K11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>42065</v>
       </c>
@@ -1576,22 +1601,22 @@
         <v>112</v>
       </c>
       <c r="E12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
         <v>140</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>146</v>
       </c>
-      <c r="I12">
-        <v>4</v>
-      </c>
-      <c r="J12">
-        <v>8</v>
-      </c>
-      <c r="K12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>42065</v>
       </c>
@@ -1605,22 +1630,22 @@
         <v>113</v>
       </c>
       <c r="E13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13">
+        <v>44</v>
+      </c>
+      <c r="G13">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
         <v>143</v>
       </c>
-      <c r="F13" t="s">
+      <c r="I13" t="s">
         <v>146</v>
       </c>
-      <c r="I13">
-        <v>44</v>
-      </c>
-      <c r="J13">
-        <v>8</v>
-      </c>
-      <c r="K13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>42067</v>
       </c>
@@ -1634,22 +1659,22 @@
         <v>114</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
-      </c>
-      <c r="F14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" t="s">
         <v>146</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>10</v>
-      </c>
-      <c r="K14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>42067</v>
       </c>
@@ -1663,22 +1688,22 @@
         <v>115</v>
       </c>
       <c r="E15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
         <v>140</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>148</v>
       </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>4</v>
-      </c>
-      <c r="K15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>42068</v>
       </c>
@@ -1692,22 +1717,22 @@
         <v>114</v>
       </c>
       <c r="E16" t="s">
+        <v>173</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
         <v>140</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>146</v>
       </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16">
-        <v>4</v>
-      </c>
-      <c r="K16" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>42068</v>
       </c>
@@ -1721,22 +1746,22 @@
         <v>116</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>141</v>
+      </c>
+      <c r="I17" t="s">
         <v>148</v>
       </c>
-      <c r="I17">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>6</v>
-      </c>
-      <c r="K17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>42068</v>
       </c>
@@ -1750,22 +1775,25 @@
         <v>117</v>
       </c>
       <c r="E18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
         <v>140</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>146</v>
       </c>
-      <c r="I18">
-        <v>7</v>
-      </c>
-      <c r="J18">
-        <v>6</v>
-      </c>
-      <c r="K18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>42069</v>
       </c>
@@ -1779,22 +1807,22 @@
         <v>118</v>
       </c>
       <c r="E19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
         <v>140</v>
       </c>
-      <c r="F19" t="s">
+      <c r="I19" t="s">
         <v>146</v>
       </c>
-      <c r="I19">
-        <v>8</v>
-      </c>
-      <c r="J19">
-        <v>8</v>
-      </c>
-      <c r="K19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>42069</v>
       </c>
@@ -1808,22 +1836,22 @@
         <v>112</v>
       </c>
       <c r="E20" t="s">
+        <v>177</v>
+      </c>
+      <c r="F20">
+        <v>27</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
         <v>143</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>146</v>
       </c>
-      <c r="I20">
-        <v>27</v>
-      </c>
-      <c r="J20">
-        <v>6</v>
-      </c>
-      <c r="K20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>42069</v>
       </c>
@@ -1837,22 +1865,22 @@
         <v>112</v>
       </c>
       <c r="E21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
         <v>140</v>
       </c>
-      <c r="F21" t="s">
+      <c r="I21" t="s">
         <v>146</v>
       </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>8</v>
-      </c>
-      <c r="K21" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>42071</v>
       </c>
@@ -1866,22 +1894,22 @@
         <v>119</v>
       </c>
       <c r="E22" t="s">
+        <v>179</v>
+      </c>
+      <c r="F22">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
         <v>140</v>
       </c>
-      <c r="F22" t="s">
+      <c r="I22" t="s">
         <v>149</v>
       </c>
-      <c r="I22">
-        <v>30</v>
-      </c>
-      <c r="J22">
-        <v>7</v>
-      </c>
-      <c r="K22" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42071</v>
       </c>
@@ -1895,22 +1923,22 @@
         <v>120</v>
       </c>
       <c r="E23" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" t="s">
+        <v>180</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" t="s">
         <v>150</v>
       </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="J23">
-        <v>6</v>
-      </c>
-      <c r="K23" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42071</v>
       </c>
@@ -1924,22 +1952,22 @@
         <v>121</v>
       </c>
       <c r="E24" t="s">
+        <v>181</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>9</v>
+      </c>
+      <c r="H24" t="s">
         <v>144</v>
       </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>146</v>
       </c>
-      <c r="I24">
-        <v>9</v>
-      </c>
-      <c r="J24">
-        <v>9</v>
-      </c>
-      <c r="K24" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42071</v>
       </c>
@@ -1953,22 +1981,22 @@
         <v>119</v>
       </c>
       <c r="E25" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" t="s">
+        <v>182</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>141</v>
+      </c>
+      <c r="I25" t="s">
         <v>146</v>
       </c>
-      <c r="I25">
-        <v>7</v>
-      </c>
-      <c r="J25">
-        <v>6</v>
-      </c>
-      <c r="K25" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>42071</v>
       </c>
@@ -1982,22 +2010,22 @@
         <v>122</v>
       </c>
       <c r="E26" t="s">
+        <v>183</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
         <v>143</v>
       </c>
-      <c r="F26" t="s">
+      <c r="I26" t="s">
         <v>146</v>
       </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>5</v>
-      </c>
-      <c r="K26" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>42072</v>
       </c>
@@ -2011,22 +2039,22 @@
         <v>123</v>
       </c>
       <c r="E27" t="s">
+        <v>184</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
         <v>143</v>
       </c>
-      <c r="F27" t="s">
+      <c r="I27" t="s">
         <v>146</v>
       </c>
-      <c r="I27">
-        <v>4</v>
-      </c>
-      <c r="J27">
-        <v>5</v>
-      </c>
-      <c r="K27" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>42387</v>
       </c>
@@ -2040,22 +2068,22 @@
         <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" t="s">
         <v>148</v>
       </c>
-      <c r="I28">
-        <v>7</v>
-      </c>
-      <c r="J28">
-        <v>25</v>
-      </c>
-      <c r="K28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43757</v>
       </c>
@@ -2069,22 +2097,22 @@
         <v>126</v>
       </c>
       <c r="E29" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
         <v>140</v>
       </c>
-      <c r="F29" t="s">
+      <c r="I29" t="s">
         <v>148</v>
       </c>
-      <c r="I29">
-        <v>8</v>
-      </c>
-      <c r="J29">
-        <v>7</v>
-      </c>
-      <c r="K29" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43757</v>
       </c>
@@ -2098,22 +2126,25 @@
         <v>127</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" t="s">
+        <v>187</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>14</v>
+      </c>
+      <c r="H30" t="s">
+        <v>141</v>
+      </c>
+      <c r="I30" t="s">
         <v>148</v>
       </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="J30">
-        <v>14</v>
-      </c>
-      <c r="K30" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44345</v>
       </c>
@@ -2127,22 +2158,22 @@
         <v>125</v>
       </c>
       <c r="E31" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>21</v>
+      </c>
+      <c r="H31" t="s">
         <v>142</v>
       </c>
-      <c r="F31" t="s">
+      <c r="I31" t="s">
         <v>146</v>
       </c>
-      <c r="I31">
-        <v>6</v>
-      </c>
-      <c r="J31">
-        <v>21</v>
-      </c>
-      <c r="K31" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45204</v>
       </c>
@@ -2156,22 +2187,22 @@
         <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" t="s">
+        <v>189</v>
+      </c>
+      <c r="F32">
+        <v>23</v>
+      </c>
+      <c r="G32">
+        <v>123</v>
+      </c>
+      <c r="H32" t="s">
+        <v>141</v>
+      </c>
+      <c r="I32" t="s">
         <v>146</v>
       </c>
-      <c r="I32">
-        <v>23</v>
-      </c>
-      <c r="J32">
-        <v>123</v>
-      </c>
-      <c r="K32" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45804</v>
       </c>
@@ -2185,22 +2216,25 @@
         <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" t="s">
+        <v>190</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="H33" t="s">
+        <v>141</v>
+      </c>
+      <c r="I33" t="s">
         <v>150</v>
       </c>
-      <c r="I33">
-        <v>8</v>
-      </c>
-      <c r="J33">
-        <v>7</v>
-      </c>
-      <c r="K33" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45805</v>
       </c>
@@ -2214,22 +2248,22 @@
         <v>130</v>
       </c>
       <c r="E34" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34" t="s">
         <v>143</v>
       </c>
-      <c r="F34" t="s">
+      <c r="I34" t="s">
         <v>146</v>
       </c>
-      <c r="I34">
-        <v>3</v>
-      </c>
-      <c r="J34">
-        <v>5</v>
-      </c>
-      <c r="K34" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>45807</v>
       </c>
@@ -2243,22 +2277,22 @@
         <v>131</v>
       </c>
       <c r="E35" t="s">
+        <v>192</v>
+      </c>
+      <c r="F35">
+        <v>37</v>
+      </c>
+      <c r="G35">
+        <v>7</v>
+      </c>
+      <c r="H35" t="s">
         <v>140</v>
       </c>
-      <c r="F35" t="s">
+      <c r="I35" t="s">
         <v>146</v>
       </c>
-      <c r="I35">
-        <v>37</v>
-      </c>
-      <c r="J35">
-        <v>7</v>
-      </c>
-      <c r="K35" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45807</v>
       </c>
@@ -2272,22 +2306,22 @@
         <v>131</v>
       </c>
       <c r="E36" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" t="s">
+        <v>193</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="H36" t="s">
+        <v>141</v>
+      </c>
+      <c r="I36" t="s">
         <v>146</v>
       </c>
-      <c r="I36">
-        <v>4</v>
-      </c>
-      <c r="J36">
-        <v>6</v>
-      </c>
-      <c r="K36" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45807</v>
       </c>
@@ -2301,25 +2335,25 @@
         <v>132</v>
       </c>
       <c r="E37" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37" t="s">
         <v>145</v>
       </c>
-      <c r="F37" t="s">
+      <c r="I37" t="s">
         <v>146</v>
       </c>
-      <c r="G37" t="s">
+      <c r="J37" t="s">
         <v>155</v>
       </c>
-      <c r="I37">
-        <v>9</v>
-      </c>
-      <c r="J37">
-        <v>4</v>
-      </c>
-      <c r="K37" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45808</v>
       </c>
@@ -2333,22 +2367,25 @@
         <v>133</v>
       </c>
       <c r="E38" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" t="s">
+        <v>195</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>6</v>
+      </c>
+      <c r="H38" t="s">
+        <v>141</v>
+      </c>
+      <c r="I38" t="s">
         <v>150</v>
       </c>
-      <c r="I38">
-        <v>3</v>
-      </c>
-      <c r="J38">
-        <v>6</v>
-      </c>
-      <c r="K38" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45808</v>
       </c>
@@ -2362,28 +2399,31 @@
         <v>134</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" t="s">
+        <v>196</v>
+      </c>
+      <c r="F39">
+        <v>66</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39" t="s">
+        <v>141</v>
+      </c>
+      <c r="I39" t="s">
         <v>150</v>
       </c>
-      <c r="G39" t="s">
+      <c r="J39" t="s">
         <v>156</v>
       </c>
-      <c r="H39" t="s">
+      <c r="K39" t="s">
         <v>152</v>
       </c>
-      <c r="I39">
-        <v>66</v>
-      </c>
-      <c r="J39">
-        <v>3</v>
-      </c>
-      <c r="K39" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45808</v>
       </c>
@@ -2397,22 +2437,25 @@
         <v>135</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>9</v>
+      </c>
+      <c r="H40" t="s">
+        <v>141</v>
+      </c>
+      <c r="I40" t="s">
         <v>150</v>
       </c>
-      <c r="I40">
-        <v>3</v>
-      </c>
-      <c r="J40">
-        <v>9</v>
-      </c>
-      <c r="K40" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45808</v>
       </c>
@@ -2426,25 +2469,28 @@
         <v>134</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41">
+        <v>27</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41" t="s">
+        <v>141</v>
+      </c>
+      <c r="I41" t="s">
         <v>150</v>
       </c>
-      <c r="H41" t="s">
+      <c r="K41" t="s">
         <v>152</v>
       </c>
-      <c r="I41">
-        <v>27</v>
-      </c>
-      <c r="J41">
-        <v>3</v>
-      </c>
-      <c r="K41" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45808</v>
       </c>
@@ -2458,25 +2504,28 @@
         <v>136</v>
       </c>
       <c r="E42" t="s">
-        <v>141</v>
-      </c>
-      <c r="F42" t="s">
+        <v>199</v>
+      </c>
+      <c r="F42">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>141</v>
+      </c>
+      <c r="I42" t="s">
         <v>149</v>
       </c>
-      <c r="G42" t="s">
+      <c r="J42" t="s">
         <v>157</v>
       </c>
-      <c r="I42">
-        <v>14</v>
-      </c>
-      <c r="J42">
-        <v>6</v>
-      </c>
-      <c r="K42" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45808</v>
       </c>
@@ -2490,22 +2539,22 @@
         <v>125</v>
       </c>
       <c r="E43" t="s">
+        <v>200</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>7</v>
+      </c>
+      <c r="H43" t="s">
         <v>145</v>
       </c>
-      <c r="F43" t="s">
+      <c r="I43" t="s">
         <v>146</v>
       </c>
-      <c r="I43">
-        <v>4</v>
-      </c>
-      <c r="J43">
-        <v>7</v>
-      </c>
-      <c r="K43" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45809</v>
       </c>
@@ -2519,22 +2568,22 @@
         <v>125</v>
       </c>
       <c r="E44" t="s">
+        <v>201</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>6</v>
+      </c>
+      <c r="H44" t="s">
         <v>145</v>
       </c>
-      <c r="F44" t="s">
+      <c r="I44" t="s">
         <v>146</v>
       </c>
-      <c r="I44">
-        <v>2</v>
-      </c>
-      <c r="J44">
-        <v>6</v>
-      </c>
-      <c r="K44" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45810</v>
       </c>
@@ -2548,22 +2597,22 @@
         <v>137</v>
       </c>
       <c r="E45" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" t="s">
+        <v>202</v>
+      </c>
+      <c r="F45">
+        <v>37</v>
+      </c>
+      <c r="G45">
+        <v>6</v>
+      </c>
+      <c r="H45" t="s">
+        <v>141</v>
+      </c>
+      <c r="I45" t="s">
         <v>148</v>
       </c>
-      <c r="I45">
-        <v>37</v>
-      </c>
-      <c r="J45">
-        <v>6</v>
-      </c>
-      <c r="K45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45810</v>
       </c>
@@ -2576,20 +2625,20 @@
       <c r="D46" t="s">
         <v>137</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46">
+        <v>5</v>
+      </c>
+      <c r="G46">
+        <v>6</v>
+      </c>
+      <c r="H46" t="s">
         <v>144</v>
       </c>
-      <c r="F46" t="s">
+      <c r="I46" t="s">
         <v>148</v>
       </c>
-      <c r="I46">
-        <v>5</v>
-      </c>
-      <c r="J46">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>45810</v>
       </c>
@@ -2603,25 +2652,25 @@
         <v>138</v>
       </c>
       <c r="E47" t="s">
-        <v>141</v>
-      </c>
-      <c r="F47" t="s">
+        <v>203</v>
+      </c>
+      <c r="F47">
+        <v>33</v>
+      </c>
+      <c r="G47">
+        <v>6</v>
+      </c>
+      <c r="H47" t="s">
+        <v>141</v>
+      </c>
+      <c r="I47" t="s">
         <v>149</v>
       </c>
-      <c r="G47" t="s">
+      <c r="J47" t="s">
         <v>158</v>
       </c>
-      <c r="I47">
-        <v>33</v>
-      </c>
-      <c r="J47">
-        <v>6</v>
-      </c>
-      <c r="K47" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45810</v>
       </c>
@@ -2635,22 +2684,22 @@
         <v>139</v>
       </c>
       <c r="E48" t="s">
+        <v>204</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>20</v>
+      </c>
+      <c r="H48" t="s">
         <v>143</v>
       </c>
-      <c r="F48" t="s">
+      <c r="I48" t="s">
         <v>151</v>
       </c>
-      <c r="I48">
-        <v>3</v>
-      </c>
-      <c r="J48">
-        <v>20</v>
-      </c>
-      <c r="K48" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>206</v>
       </c>
@@ -2664,16 +2713,16 @@
         <v>113</v>
       </c>
       <c r="E49" t="s">
-        <v>141</v>
-      </c>
-      <c r="I49">
+        <v>208</v>
+      </c>
+      <c r="F49">
         <v>3</v>
       </c>
-      <c r="K49" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>210</v>
       </c>
@@ -2687,16 +2736,16 @@
         <v>113</v>
       </c>
       <c r="E50" t="s">
-        <v>141</v>
-      </c>
-      <c r="I50">
+        <v>212</v>
+      </c>
+      <c r="F50">
         <v>1</v>
       </c>
-      <c r="K50" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>210</v>
       </c>
@@ -2710,16 +2759,16 @@
         <v>215</v>
       </c>
       <c r="E51" t="s">
-        <v>141</v>
-      </c>
-      <c r="I51">
+        <v>216</v>
+      </c>
+      <c r="F51">
         <v>8</v>
       </c>
-      <c r="K51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>210</v>
       </c>
@@ -2733,16 +2782,16 @@
         <v>113</v>
       </c>
       <c r="E52" t="s">
-        <v>141</v>
-      </c>
-      <c r="I52">
+        <v>212</v>
+      </c>
+      <c r="F52">
         <v>1</v>
       </c>
-      <c r="K52" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>220</v>
       </c>
@@ -2756,16 +2805,16 @@
         <v>222</v>
       </c>
       <c r="E53" t="s">
-        <v>141</v>
-      </c>
-      <c r="I53">
+        <v>223</v>
+      </c>
+      <c r="F53">
         <v>5</v>
       </c>
-      <c r="K53" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>210</v>
       </c>
@@ -2779,16 +2828,16 @@
         <v>113</v>
       </c>
       <c r="E54" t="s">
-        <v>141</v>
-      </c>
-      <c r="I54">
+        <v>212</v>
+      </c>
+      <c r="F54">
         <v>3</v>
       </c>
-      <c r="K54" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>210</v>
       </c>
@@ -2802,16 +2851,16 @@
         <v>113</v>
       </c>
       <c r="E55" t="s">
-        <v>141</v>
-      </c>
-      <c r="I55">
+        <v>212</v>
+      </c>
+      <c r="F55">
         <v>2</v>
       </c>
-      <c r="K55" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>210</v>
       </c>
@@ -2825,16 +2874,16 @@
         <v>230</v>
       </c>
       <c r="E56" t="s">
-        <v>141</v>
-      </c>
-      <c r="I56">
+        <v>231</v>
+      </c>
+      <c r="F56">
         <v>3</v>
       </c>
-      <c r="K56" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>210</v>
       </c>
@@ -2848,16 +2897,16 @@
         <v>113</v>
       </c>
       <c r="E57" t="s">
-        <v>141</v>
-      </c>
-      <c r="I57">
+        <v>234</v>
+      </c>
+      <c r="F57">
         <v>2</v>
       </c>
-      <c r="K57" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H57" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>236</v>
       </c>
@@ -2871,16 +2920,16 @@
         <v>238</v>
       </c>
       <c r="E58" t="s">
-        <v>141</v>
-      </c>
-      <c r="I58">
+        <v>239</v>
+      </c>
+      <c r="F58">
         <v>8</v>
       </c>
-      <c r="K58" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>241</v>
       </c>
@@ -2894,16 +2943,16 @@
         <v>113</v>
       </c>
       <c r="E59" t="s">
-        <v>141</v>
-      </c>
-      <c r="I59">
+        <v>208</v>
+      </c>
+      <c r="F59">
         <v>10</v>
       </c>
-      <c r="K59" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>244</v>
       </c>
@@ -2917,13 +2966,13 @@
         <v>246</v>
       </c>
       <c r="E60" t="s">
-        <v>141</v>
-      </c>
-      <c r="I60">
+        <v>247</v>
+      </c>
+      <c r="F60">
         <v>5</v>
       </c>
-      <c r="K60" t="s">
-        <v>247</v>
+      <c r="H60" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>